<commit_message>
added binary search tree implementation
</commit_message>
<xml_diff>
--- a/OOP/CSC_517/dogsv1.xlsx
+++ b/OOP/CSC_517/dogsv1.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
@@ -527,6 +527,26 @@
       </c>
       <c r="B7" s="2" t="n">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Dingo</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Gerbbbbb</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>